<commit_message>
added time measurement, streets with EasyRoads3D
</commit_message>
<xml_diff>
--- a/Checkpoints.xlsx
+++ b/Checkpoints.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Buggy Modell in Blender aufbereiten (im Minimum losgelöste Räder)</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>UV Mapping nicht funktioniert</t>
+  </si>
+  <si>
+    <t>rateOverDistance statt rate!</t>
+  </si>
+  <si>
+    <t>Zusätzlich Checkpoints hinzugefügt</t>
+  </si>
+  <si>
+    <t>Optional: Asphaltierte Strassen mit EasyRoad</t>
   </si>
 </sst>
 </file>
@@ -514,16 +523,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -717,7 +726,7 @@
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="6"/>
@@ -730,8 +739,13 @@
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="D19" s="6"/>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -758,8 +772,13 @@
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="D22" s="6"/>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
@@ -779,7 +798,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>8</v>
       </c>
@@ -789,7 +808,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" t="s">
         <v>29</v>
@@ -797,21 +816,31 @@
       <c r="C26" s="3"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A16:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="D16:D27"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="D16:D28"/>
     <mergeCell ref="D3:D15"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A1:C1"/>

</xml_diff>